<commit_message>
Changed HL7 mappings for hospitalization prediction model
</commit_message>
<xml_diff>
--- a/legacy/MirthConnect/Model1 AI Guesses.xlsx
+++ b/legacy/MirthConnect/Model1 AI Guesses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Guedes\Desktop\Git Repos\ABI-Interoperability\MirthConnect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Guedes\Desktop\Git Repos\Tese\ABI-Interoperability\legacy\MirthConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA09E47-E28E-4154-A969-800D882FCF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A68511-000A-4128-9078-B886C6BF7DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DBE87373-5EFC-4536-A5EA-32B1C8DD87E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>HORA_ADMISSAO</t>
   </si>
@@ -236,6 +236,12 @@
   <si>
     <t>OBX-3.1 (identifier)
 OBX-5.1 (color)</t>
+  </si>
+  <si>
+    <t>Parse Date and / 1000</t>
+  </si>
+  <si>
+    <t>Preprocessing of Direct mapping</t>
   </si>
 </sst>
 </file>
@@ -632,23 +638,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADA39CE-2A6C-4A74-B40F-85860EE19204}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -674,7 +680,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -700,7 +706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -714,7 +720,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>40</v>
@@ -726,7 +732,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -740,7 +746,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>40</v>
@@ -752,7 +758,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -765,7 +771,7 @@
       <c r="D5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -778,7 +784,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -804,7 +810,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -830,7 +836,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -856,7 +862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -882,7 +888,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -908,7 +914,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -935,7 +941,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -962,7 +968,7 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -971,7 +977,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished version 1 final
</commit_message>
<xml_diff>
--- a/legacy/MirthConnect/Model1 AI Guesses.xlsx
+++ b/legacy/MirthConnect/Model1 AI Guesses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao Guedes\Desktop\Git Repos\Tese\ABI-Interoperability\legacy\MirthConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A68511-000A-4128-9078-B886C6BF7DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D91886-58FB-4F45-8671-7F3779234D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DBE87373-5EFC-4536-A5EA-32B1C8DD87E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>HORA_ADMISSAO</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>https://hl7-definition.caristix.com/v2/HL7v2.4/Fields/DG1.3.1</t>
-  </si>
-  <si>
-    <t>Consulting Doctor</t>
   </si>
   <si>
     <t>https://hl7-definition.caristix.com/v2/HL7v2.4/Fields/PV1.9</t>
@@ -216,9 +213,6 @@
     <t>Observation Identifier / Observation Value</t>
   </si>
   <si>
-    <t>value * 86400</t>
-  </si>
-  <si>
     <t>PV1-19.1</t>
   </si>
   <si>
@@ -226,9 +220,6 @@
   </si>
   <si>
     <t>DG1-3.1</t>
-  </si>
-  <si>
-    <t>PV1-9.1</t>
   </si>
   <si>
     <t>PID-8.1</t>
@@ -238,10 +229,22 @@
 OBX-5.1 (color)</t>
   </si>
   <si>
-    <t>Parse Date and / 1000</t>
-  </si>
-  <si>
-    <t>Preprocessing of Direct mapping</t>
+    <t>preprocessing table</t>
+  </si>
+  <si>
+    <t>PV1-9.7</t>
+  </si>
+  <si>
+    <t>Consulting Doctor Degree</t>
+  </si>
+  <si>
+    <t>preprocessing table (hl7 docs)</t>
+  </si>
+  <si>
+    <t>Direct mapping * 86400</t>
+  </si>
+  <si>
+    <t>Direct mapping / 1000</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -321,6 +324,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -639,7 +645,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,6 +658,7 @@
     <col min="6" max="6" width="28.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="58" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -688,7 +695,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>24</v>
@@ -705,6 +712,7 @@
       <c r="H2" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -714,13 +722,13 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>40</v>
@@ -740,13 +748,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>40</v>
@@ -766,13 +774,13 @@
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>65</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>40</v>
@@ -781,7 +789,7 @@
         <v>42</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -798,7 +806,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>40</v>
@@ -807,7 +815,7 @@
         <v>42</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -833,7 +841,7 @@
         <v>42</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -844,13 +852,13 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>43</v>
@@ -859,7 +867,7 @@
         <v>44</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -870,13 +878,13 @@
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>40</v>
@@ -885,7 +893,7 @@
         <v>42</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -896,13 +904,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>40</v>
@@ -911,7 +919,7 @@
         <v>42</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -922,10 +930,10 @@
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>31</v>
@@ -937,7 +945,7 @@
         <v>44</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L11" s="1"/>
     </row>
@@ -949,13 +957,13 @@
         <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>40</v>
@@ -964,7 +972,7 @@
         <v>42</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N12" s="1"/>
     </row>

</xml_diff>